<commit_message>
added .pin file avg 6% error in numbers at length
</commit_message>
<xml_diff>
--- a/not_gmacs_2/fiddling with parameters.xlsx
+++ b/not_gmacs_2/fiddling with parameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Desktop\snow20\not_gmacs_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gmacs_term\not_gmacs_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10596" windowHeight="7020" tabRatio="684" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10596" windowHeight="7020" tabRatio="684" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2016sc" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="152">
   <si>
     <t># Number of parameters = 327 Objective function value = 7766.45  Maximum gradient component = 0.00411848</t>
   </si>
@@ -459,6 +459,27 @@
   </si>
   <si>
     <t>fem_mat</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>old code</t>
+  </si>
+  <si>
+    <t>len bin</t>
+  </si>
+  <si>
+    <t>in_alpha</t>
+  </si>
+  <si>
+    <t>devia</t>
+  </si>
+  <si>
+    <t>reclen</t>
   </si>
 </sst>
 </file>
@@ -2204,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2627,6 +2648,12 @@
       <c r="C21">
         <v>11.801595789</v>
       </c>
+      <c r="E21">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F21">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22">
@@ -2635,6 +2662,12 @@
       <c r="C22">
         <v>11.7595130617</v>
       </c>
+      <c r="E22">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F22">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23">
@@ -2643,6 +2676,12 @@
       <c r="C23">
         <v>11.607895517499999</v>
       </c>
+      <c r="E23">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F23">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24">
@@ -2651,6 +2690,12 @@
       <c r="C24">
         <v>11.275088521200001</v>
       </c>
+      <c r="E24">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F24">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25">
@@ -2659,6 +2704,12 @@
       <c r="C25">
         <v>10.6175423654</v>
       </c>
+      <c r="E25">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F25">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26">
@@ -2667,6 +2718,12 @@
       <c r="C26">
         <v>9.7123235722899999</v>
       </c>
+      <c r="E26">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F26">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27">
@@ -2675,6 +2732,12 @@
       <c r="C27">
         <v>8.6431693632099993</v>
       </c>
+      <c r="E27">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F27">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28">
@@ -2683,6 +2746,12 @@
       <c r="C28">
         <v>7.47839448604</v>
       </c>
+      <c r="E28">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F28">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29">
@@ -2691,6 +2760,12 @@
       <c r="C29">
         <v>6.2718374921900004</v>
       </c>
+      <c r="E29">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F29">
+        <v>-9.8999579077799993</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30">
@@ -2698,6 +2773,12 @@
       </c>
       <c r="C30">
         <v>5.0551975606799999</v>
+      </c>
+      <c r="E30">
+        <v>-9.8999579077799993</v>
+      </c>
+      <c r="F30">
+        <v>-9.8999579077799993</v>
       </c>
     </row>
   </sheetData>
@@ -2709,7 +2790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -3338,76 +3419,393 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>122</v>
       </c>
       <c r="B1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>27.5</v>
       </c>
       <c r="B2">
         <v>0.155832</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>27.5</v>
+      </c>
+      <c r="E2">
+        <f>D2+2.5-$D$2</f>
+        <v>2.5</v>
+      </c>
+      <c r="F2">
+        <f>(E2^($J$4-1))*EXP(-E2/$J$2)</f>
+        <v>2.9833449046478431</v>
+      </c>
+      <c r="G2">
+        <f>F2/$F$24</f>
+        <v>0.1558317289228196</v>
+      </c>
+      <c r="I2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>32.5</v>
       </c>
       <c r="B3">
         <v>0.35026000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>32.5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E23" si="0">D3+2.5-$D$2</f>
+        <v>7.5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F14" si="1">(E3^($J$4-1))*EXP(-E3/$J$2)</f>
+        <v>6.705601108624041</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="2">F3/$F$24</f>
+        <v>0.3502596741649644</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>37.5</v>
       </c>
       <c r="B4">
         <v>0.26151000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>37.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>5.0065207265136253</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0.26151008536930859</v>
+      </c>
+      <c r="I4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J4">
+        <f>J1/J2</f>
+        <v>2.875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>42.5</v>
       </c>
       <c r="B5">
         <v>0.14080300000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>42.5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>2.6956157360228947</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0.14080251331368981</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>47.5</v>
       </c>
       <c r="B6">
         <v>6.4623200000000006E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>47.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1.2371881760627037</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>6.4623159118599588E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>52.5</v>
       </c>
       <c r="B7">
         <v>2.6972800000000002E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>52.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>27.5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.51638573659414322</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>2.6972839110618263E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>57.5</v>
       </c>
       <c r="B8">
         <v>0</v>
+      </c>
+      <c r="D8">
+        <v>57.5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>32.5</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>62.5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>37.5</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>67.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>42.5</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>72.5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>47.5</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>77.5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>82.5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>57.5</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>87.5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>62.5</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>92.5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>67.5</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>97.5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>72.5</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>102.5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>107.5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>82.5</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>112.5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>117.5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>122.5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>97.5</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>127.5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>102.5</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>132.5</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>107.5</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f>SUM(F2:F23)</f>
+        <v>19.144656388465247</v>
       </c>
     </row>
   </sheetData>
@@ -3512,8 +3910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added immature/mature natural mortality corrected logistic selectivity--was denoted as logistic95 commented out code that normalized selectivity based on the terminal size bin
</commit_message>
<xml_diff>
--- a/not_gmacs_2/fiddling with parameters.xlsx
+++ b/not_gmacs_2/fiddling with parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10596" windowHeight="7020" tabRatio="684" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10596" windowHeight="7020" tabRatio="684"/>
   </bookViews>
   <sheets>
     <sheet name="2016sc" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,41 @@
     <sheet name="Natural mortality" sheetId="5" r:id="rId5"/>
     <sheet name="maturity" sheetId="2" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'Natural mortality'!$D$9</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'Natural mortality'!$E$9</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0.322415</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="159">
   <si>
     <t># Number of parameters = 327 Objective function value = 7766.45  Maximum gradient component = 0.00411848</t>
   </si>
@@ -480,6 +509,27 @@
   </si>
   <si>
     <t>reclen</t>
+  </si>
+  <si>
+    <t>mature male</t>
+  </si>
+  <si>
+    <t>mature female</t>
+  </si>
+  <si>
+    <t>needed multiplier</t>
+  </si>
+  <si>
+    <t>maturity_est</t>
+  </si>
+  <si>
+    <t>mat_new</t>
+  </si>
+  <si>
+    <t>mat_old</t>
+  </si>
+  <si>
+    <t>imm_new</t>
   </si>
 </sst>
 </file>
@@ -1297,13 +1347,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:R177"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:A63"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1705,12 +1758,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>0.50000005000000003</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>53</v>
       </c>
@@ -1718,7 +1771,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4.6607123776700004</v>
       </c>
@@ -1727,143 +1780,365 @@
         <v>105.71136175330247</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4.5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>57</v>
       </c>
       <c r="C90" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>0.200110432177</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <f>1/A91</f>
+        <v>4.9972407191419608</v>
+      </c>
+      <c r="D91">
+        <f>LN(C91)</f>
+        <v>1.6088859039338306</v>
+      </c>
+      <c r="G91">
+        <v>27.5</v>
+      </c>
+      <c r="H91">
+        <f>1/(1+EXP(-$A$95*(G91-$A$97)))</f>
+        <v>2.8329918833784871E-14</v>
+      </c>
+      <c r="J91" s="1">
+        <v>4.5412700000000001E-21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G92">
+        <v>32.5</v>
+      </c>
+      <c r="H92">
+        <f t="shared" ref="H92:H112" si="0">1/(1+EXP(-$A$95*(G92-$A$97)))</f>
+        <v>2.7578275686439838E-13</v>
+      </c>
+      <c r="J92" s="1">
+        <v>1.2023599999999999E-19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G93">
+        <v>37.5</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="0"/>
+        <v>2.6846574968955772E-12</v>
+      </c>
+      <c r="J93" s="1">
+        <v>3.1833800000000001E-18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C94" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G94">
+        <v>42.5</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="0"/>
+        <v>2.6134287572699125E-11</v>
+      </c>
+      <c r="J94" s="1">
+        <v>8.4283800000000004E-17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>0.45513899883199999</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <f>1/A95</f>
+        <v>2.1971309919963988</v>
+      </c>
+      <c r="D95">
+        <f>LN(C95)</f>
+        <v>0.78715241474588604</v>
+      </c>
+      <c r="G95">
+        <v>47.5</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="0"/>
+        <v>2.5440898423073917E-10</v>
+      </c>
+      <c r="J95" s="1">
+        <v>2.2315000000000001E-15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G96">
+        <v>52.5</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="0"/>
+        <v>2.4765906071943536E-9</v>
+      </c>
+      <c r="J96" s="1">
+        <v>5.9080900000000001E-14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96.0391891843</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <f>LN(A97)</f>
+        <v>4.5647563288382393</v>
+      </c>
+      <c r="G97">
+        <v>57.5</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="0"/>
+        <v>2.4108822002248582E-8</v>
+      </c>
+      <c r="J97" s="1">
+        <v>1.5641799999999999E-12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G98">
+        <v>62.5</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="0"/>
+        <v>2.3469167121238143E-7</v>
+      </c>
+      <c r="J98" s="1">
+        <v>4.1408900000000001E-11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>0.27500000000000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G99">
+        <v>67.5</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="0"/>
+        <v>2.2846441530185272E-6</v>
+      </c>
+      <c r="J99" s="1">
+        <v>1.0960199999999999E-9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G100">
+        <v>72.5</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="0"/>
+        <v>2.2239840980882428E-5</v>
+      </c>
+      <c r="J100" s="1">
+        <v>2.8994000000000001E-8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G101">
+        <v>77.5</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="0"/>
+        <v>2.1645573608994887E-4</v>
+      </c>
+      <c r="J101" s="1">
+        <v>7.6579399999999998E-7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G102">
+        <v>82.5</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="0"/>
+        <v>2.1031514335649874E-3</v>
+      </c>
+      <c r="J102" s="1">
+        <v>2.01152E-5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G103">
+        <v>87.5</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="0"/>
+        <v>2.0104189654354995E-2</v>
+      </c>
+      <c r="J103">
+        <v>5.1454500000000004E-4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G104">
+        <v>92.5</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="0"/>
+        <v>0.16647437914588792</v>
+      </c>
+      <c r="J104">
+        <v>1.11019E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>159.5</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G105">
+        <v>97.5</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="0"/>
+        <v>0.6603539587344629</v>
+      </c>
+      <c r="J105">
+        <v>0.107502</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G106">
+        <v>102.5</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="0"/>
+        <v>0.94981575859577216</v>
+      </c>
+      <c r="J106">
+        <v>0.32889499999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1.0049999999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G107">
+        <v>107.5</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="0"/>
+        <v>0.99460171983439971</v>
+      </c>
+      <c r="J107">
+        <v>0.58811100000000005</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G108">
+        <v>112.5</v>
+      </c>
+      <c r="H108">
+        <f t="shared" si="0"/>
+        <v>0.99944275989909015</v>
+      </c>
+      <c r="J108">
+        <v>0.79880399999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>130</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G109">
+        <v>117.5</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="0"/>
+        <v>0.99994272860203715</v>
+      </c>
+      <c r="J109">
+        <v>0.91788899999999995</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>67</v>
       </c>
@@ -1871,22 +2146,59 @@
       <c r="C110" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G110">
+        <v>122.5</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="0"/>
+        <v>0.99999411646523695</v>
+      </c>
+      <c r="J110">
+        <v>0.97095100000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>0.23881599579099999</v>
       </c>
       <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C111" s="2">
+        <f>1/A111</f>
+        <v>4.187324206185715</v>
+      </c>
+      <c r="D111">
+        <f>LN(C111)</f>
+        <v>1.4320619156576078</v>
+      </c>
+      <c r="G111">
+        <v>127.5</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="0"/>
+        <v>0.9999993956078177</v>
+      </c>
+      <c r="J111">
+        <v>0.99202199999999996</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G112">
+        <v>132.5</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="0"/>
+        <v>0.99999993791348329</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>4.3155758708500001</v>
       </c>
@@ -1896,157 +2208,829 @@
       </c>
       <c r="C113" s="2"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>8.42583821087E-2</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <f>1/A117</f>
+        <v>11.868255418314591</v>
+      </c>
+      <c r="D117">
+        <f>LN(C117)</f>
+        <v>2.4738672237941066</v>
+      </c>
+      <c r="E117">
+        <v>25</v>
+      </c>
+      <c r="F117">
+        <v>27.5</v>
+      </c>
+      <c r="G117">
+        <f>1/(1+EXP(-$A$117*(F117-$A$119)))</f>
+        <v>9.6203133200029468E-4</v>
+      </c>
+      <c r="H117">
+        <f>1/(1+EXP(-(F117-$A$119)/$C$117))</f>
+        <v>9.6203133200029468E-4</v>
+      </c>
+      <c r="I117">
+        <f>H117/$H$138</f>
+        <v>1.1056868133211917E-3</v>
+      </c>
+      <c r="K117">
+        <f>LN(H117)</f>
+        <v>-6.946463538182071</v>
+      </c>
+      <c r="L117">
+        <f>K117-$K$138</f>
+        <v>-6.807288586578025</v>
+      </c>
+      <c r="M117">
+        <f>EXP(L117)</f>
+        <v>1.1056868133211917E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E118">
+        <v>30</v>
+      </c>
+      <c r="F118">
+        <v>32.5</v>
+      </c>
+      <c r="G118">
+        <f t="shared" ref="G118:G138" si="1">1/(1+EXP(-$A$117*(F118-$A$119)))</f>
+        <v>1.4653289289554936E-3</v>
+      </c>
+      <c r="H118">
+        <f t="shared" ref="H118:H130" si="2">1/(1+EXP(-(F118-$A$119)/$C$117))</f>
+        <v>1.4653289289554936E-3</v>
+      </c>
+      <c r="I118">
+        <f t="shared" ref="I118:I138" si="3">H118/$H$138</f>
+        <v>1.6841394038127424E-3</v>
+      </c>
+      <c r="K118">
+        <f t="shared" ref="K118:K138" si="4">LN(H118)</f>
+        <v>-6.5256755368307502</v>
+      </c>
+      <c r="L118">
+        <f t="shared" ref="L118:L138" si="5">K118-$K$138</f>
+        <v>-6.3865005852267043</v>
+      </c>
+      <c r="M118">
+        <f t="shared" ref="M118:M138" si="6">EXP(L118)</f>
+        <v>1.6841394038127418E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>109.930980396</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C119">
+        <f>LN(A119)</f>
+        <v>4.6998527179172367</v>
+      </c>
+      <c r="E119">
+        <v>35</v>
+      </c>
+      <c r="F119">
+        <v>37.5</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="1"/>
+        <v>2.2313442774069166E-3</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="2"/>
+        <v>2.2313442774069166E-3</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="3"/>
+        <v>2.5645401157347912E-3</v>
+      </c>
+      <c r="K119">
+        <f t="shared" si="4"/>
+        <v>-6.105151060149395</v>
+      </c>
+      <c r="L119">
+        <f t="shared" si="5"/>
+        <v>-5.9659761085453491</v>
+      </c>
+      <c r="M119">
+        <f t="shared" si="6"/>
+        <v>2.5645401157347899E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E120">
+        <v>40</v>
+      </c>
+      <c r="F120">
+        <v>42.5</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="1"/>
+        <v>3.3964397345092375E-3</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="2"/>
+        <v>3.3964397345092375E-3</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="3"/>
+        <v>3.9036136368642131E-3</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="4"/>
+        <v>-5.6850275328999498</v>
+      </c>
+      <c r="L120">
+        <f t="shared" si="5"/>
+        <v>-5.5458525812959039</v>
+      </c>
+      <c r="M120">
+        <f t="shared" si="6"/>
+        <v>3.9036136368642135E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E121">
+        <v>45</v>
+      </c>
+      <c r="F121">
+        <v>47.5</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="1"/>
+        <v>5.16673904855068E-3</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="2"/>
+        <v>5.16673904855068E-3</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="3"/>
+        <v>5.9382631769132627E-3</v>
+      </c>
+      <c r="K121">
+        <f t="shared" si="4"/>
+        <v>-5.2655135344262707</v>
+      </c>
+      <c r="L121">
+        <f t="shared" si="5"/>
+        <v>-5.1263385828222248</v>
+      </c>
+      <c r="M121">
+        <f t="shared" si="6"/>
+        <v>5.9382631769132619E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E122">
+        <v>50</v>
+      </c>
+      <c r="F122">
+        <v>52.5</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="1"/>
+        <v>7.8524870846216066E-3</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="2"/>
+        <v>7.8524870846216066E-3</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="3"/>
+        <v>9.0250609646863565E-3</v>
+      </c>
+      <c r="K122">
+        <f t="shared" si="4"/>
+        <v>-4.8469249713001528</v>
+      </c>
+      <c r="L122">
+        <f t="shared" si="5"/>
+        <v>-4.7077500196961068</v>
+      </c>
+      <c r="M122">
+        <f t="shared" si="6"/>
+        <v>9.0250609646863583E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E123">
+        <v>55</v>
+      </c>
+      <c r="F123">
+        <v>57.5</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="1"/>
+        <v>1.1917602537126579E-2</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="2"/>
+        <v>1.1917602537126579E-2</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="3"/>
+        <v>1.3697200427251782E-2</v>
+      </c>
+      <c r="K123">
+        <f t="shared" si="4"/>
+        <v>-4.4297387670098605</v>
+      </c>
+      <c r="L123">
+        <f t="shared" si="5"/>
+        <v>-4.2905638154058146</v>
+      </c>
+      <c r="M123">
+        <f t="shared" si="6"/>
+        <v>1.3697200427251779E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E124">
+        <v>60</v>
+      </c>
+      <c r="F124">
+        <v>62.5</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="1"/>
+        <v>1.8048884043698876E-2</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="2"/>
+        <v>1.8048884043698876E-2</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="3"/>
+        <v>2.0744036517799196E-2</v>
+      </c>
+      <c r="K124">
+        <f t="shared" si="4"/>
+        <v>-4.0146714219483997</v>
+      </c>
+      <c r="L124">
+        <f t="shared" si="5"/>
+        <v>-3.8754964703443537</v>
+      </c>
+      <c r="M124">
+        <f t="shared" si="6"/>
+        <v>2.07440365177992E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>60</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E125">
+        <v>65</v>
+      </c>
+      <c r="F125">
+        <v>67.5</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="1"/>
+        <v>2.7247556950463242E-2</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="2"/>
+        <v>2.7247556950463242E-2</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="3"/>
+        <v>3.1316302716153287E-2</v>
+      </c>
+      <c r="K125">
+        <f t="shared" si="4"/>
+        <v>-3.6027914150859814</v>
+      </c>
+      <c r="L125">
+        <f t="shared" si="5"/>
+        <v>-3.4636164634819355</v>
+      </c>
+      <c r="M125">
+        <f t="shared" si="6"/>
+        <v>3.1316302716153273E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E126">
+        <v>70</v>
+      </c>
+      <c r="F126">
+        <v>72.5</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="1"/>
+        <v>4.0938908828684985E-2</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="2"/>
+        <v>4.0938908828684985E-2</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="3"/>
+        <v>4.7052117886345141E-2</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="4"/>
+        <v>-3.1956743520430027</v>
+      </c>
+      <c r="L126">
+        <f t="shared" si="5"/>
+        <v>-3.0564994004389563</v>
+      </c>
+      <c r="M126">
+        <f t="shared" si="6"/>
+        <v>4.7052117886345154E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>40</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E127">
+        <v>75</v>
+      </c>
+      <c r="F127">
+        <v>77.5</v>
+      </c>
+      <c r="G127">
+        <f t="shared" si="1"/>
+        <v>6.1077927422646811E-2</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="2"/>
+        <v>6.1077927422646811E-2</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="3"/>
+        <v>7.0198398627820055E-2</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="4"/>
+        <v>-2.7956047313841204</v>
+      </c>
+      <c r="L127">
+        <f t="shared" si="5"/>
+        <v>-2.6564297797800744</v>
+      </c>
+      <c r="M127">
+        <f t="shared" si="6"/>
+        <v>7.0198398627820041E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E128">
+        <v>80</v>
+      </c>
+      <c r="F128">
+        <v>82.5</v>
+      </c>
+      <c r="G128">
+        <f t="shared" si="1"/>
+        <v>9.0192232146976789E-2</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="2"/>
+        <v>9.0192232146976789E-2</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="3"/>
+        <v>0.10366020152541702</v>
+      </c>
+      <c r="K128">
+        <f t="shared" si="4"/>
+        <v>-2.4058119737264061</v>
+      </c>
+      <c r="L128">
+        <f t="shared" si="5"/>
+        <v>-2.2666370221223602</v>
+      </c>
+      <c r="M128">
+        <f t="shared" si="6"/>
+        <v>0.10366020152541701</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>0.44649064771300001</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E129">
+        <v>85</v>
+      </c>
+      <c r="F129">
+        <v>87.5</v>
+      </c>
+      <c r="G129">
+        <f t="shared" si="1"/>
+        <v>0.13124468410532175</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="2"/>
+        <v>0.13124468410532175</v>
+      </c>
+      <c r="I129">
+        <f t="shared" si="3"/>
+        <v>0.15084281738727739</v>
+      </c>
+      <c r="K129">
+        <f t="shared" si="4"/>
+        <v>-2.0306918803853256</v>
+      </c>
+      <c r="L129">
+        <f t="shared" si="5"/>
+        <v>-1.8915169287812794</v>
+      </c>
+      <c r="M129">
+        <f t="shared" si="6"/>
+        <v>0.15084281738727742</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E130">
+        <v>90</v>
+      </c>
+      <c r="F130">
+        <v>92.5</v>
+      </c>
+      <c r="G130">
+        <f t="shared" si="1"/>
+        <v>0.18713934382416181</v>
+      </c>
+      <c r="H130">
+        <f t="shared" si="2"/>
+        <v>0.18713934382416181</v>
+      </c>
+      <c r="I130">
+        <f t="shared" si="3"/>
+        <v>0.21508395603885896</v>
+      </c>
+      <c r="K130">
+        <f t="shared" si="4"/>
+        <v>-1.6759017854771541</v>
+      </c>
+      <c r="L130">
+        <f t="shared" si="5"/>
+        <v>-1.5367268338731079</v>
+      </c>
+      <c r="M130">
+        <f t="shared" si="6"/>
+        <v>0.21508395603885896</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>0.52016917924799999</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E131">
+        <v>95</v>
+      </c>
+      <c r="F131">
+        <v>97.5</v>
+      </c>
+      <c r="G131">
+        <f t="shared" si="1"/>
+        <v>0.25972193596031634</v>
+      </c>
+      <c r="H131">
+        <f t="shared" ref="H131:H138" si="7">1/(1+EXP(-(F131-$A$119)/$C$117))</f>
+        <v>0.25972193596031634</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="3"/>
+        <v>0.29850495526426873</v>
+      </c>
+      <c r="K131">
+        <f t="shared" si="4"/>
+        <v>-1.3481436973409999</v>
+      </c>
+      <c r="L131">
+        <f t="shared" si="5"/>
+        <v>-1.2089687457369538</v>
+      </c>
+      <c r="M131">
+        <f t="shared" si="6"/>
+        <v>0.29850495526426873</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E132">
+        <v>100</v>
+      </c>
+      <c r="F132">
+        <v>102.5</v>
+      </c>
+      <c r="G132">
+        <f t="shared" si="1"/>
+        <v>0.34839029418223494</v>
+      </c>
+      <c r="H132">
+        <f t="shared" si="7"/>
+        <v>0.34839029418223494</v>
+      </c>
+      <c r="I132">
+        <f t="shared" si="3"/>
+        <v>0.40041373014893644</v>
+      </c>
+      <c r="K132">
+        <f t="shared" si="4"/>
+        <v>-1.0544318926517835</v>
+      </c>
+      <c r="L132">
+        <f t="shared" si="5"/>
+        <v>-0.91525694104773736</v>
+      </c>
+      <c r="M132">
+        <f t="shared" si="6"/>
+        <v>0.40041373014893644</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>63.216811077099997</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E133">
+        <v>105</v>
+      </c>
+      <c r="F133">
+        <v>107.5</v>
+      </c>
+      <c r="G133">
+        <f t="shared" si="1"/>
+        <v>0.44897067011196212</v>
+      </c>
+      <c r="H133">
+        <f t="shared" si="7"/>
+        <v>0.44897067011196212</v>
+      </c>
+      <c r="I133">
+        <f t="shared" si="3"/>
+        <v>0.51601328667601376</v>
+      </c>
+      <c r="K133">
+        <f t="shared" si="4"/>
+        <v>-0.80079771606401018</v>
+      </c>
+      <c r="L133">
+        <f t="shared" si="5"/>
+        <v>-0.66162276445996404</v>
+      </c>
+      <c r="M133">
+        <f t="shared" si="6"/>
+        <v>0.51601328667601376</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E134">
+        <v>110</v>
+      </c>
+      <c r="F134">
+        <v>112.5</v>
+      </c>
+      <c r="G134">
+        <f t="shared" si="1"/>
+        <v>0.5539050438251869</v>
+      </c>
+      <c r="H134">
+        <f t="shared" si="7"/>
+        <v>0.5539050438251869</v>
+      </c>
+      <c r="I134">
+        <f t="shared" si="3"/>
+        <v>0.63661700239656893</v>
+      </c>
+      <c r="K134">
+        <f t="shared" si="4"/>
+        <v>-0.59076200796325851</v>
+      </c>
+      <c r="L134">
+        <f t="shared" si="5"/>
+        <v>-0.45158705635921237</v>
+      </c>
+      <c r="M134">
+        <f t="shared" si="6"/>
+        <v>0.63661700239656893</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>42.190179705299997</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E135">
+        <v>115</v>
+      </c>
+      <c r="F135">
+        <v>117.5</v>
+      </c>
+      <c r="G135">
+        <f t="shared" si="1"/>
+        <v>0.65424542497681171</v>
+      </c>
+      <c r="H135">
+        <f t="shared" si="7"/>
+        <v>0.65424542497681171</v>
+      </c>
+      <c r="I135">
+        <f t="shared" si="3"/>
+        <v>0.75194072688721769</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="4"/>
+        <v>-0.42427273037155233</v>
+      </c>
+      <c r="L135">
+        <f t="shared" si="5"/>
+        <v>-0.28509777876750619</v>
+      </c>
+      <c r="M135">
+        <f t="shared" si="6"/>
+        <v>0.75194072688721758</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E136">
+        <v>120</v>
+      </c>
+      <c r="F136">
+        <v>122.5</v>
+      </c>
+      <c r="G136">
+        <f t="shared" si="1"/>
+        <v>0.74250805031275724</v>
+      </c>
+      <c r="H136">
+        <f t="shared" si="7"/>
+        <v>0.74250805031275724</v>
+      </c>
+      <c r="I136">
+        <f t="shared" si="3"/>
+        <v>0.85338318275832648</v>
+      </c>
+      <c r="K136">
+        <f t="shared" si="4"/>
+        <v>-0.29772156619199469</v>
+      </c>
+      <c r="L136">
+        <f t="shared" si="5"/>
+        <v>-0.15854661458794855</v>
+      </c>
+      <c r="M136">
+        <f t="shared" si="6"/>
+        <v>0.85338318275832636</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>0.784139414516</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E137">
+        <v>125</v>
+      </c>
+      <c r="F137">
+        <v>127.5</v>
+      </c>
+      <c r="G137">
+        <f t="shared" si="1"/>
+        <v>0.81462350239922254</v>
+      </c>
+      <c r="H137">
+        <f t="shared" si="7"/>
+        <v>0.81462350239922254</v>
+      </c>
+      <c r="I137">
+        <f t="shared" si="3"/>
+        <v>0.93626728617199417</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="4"/>
+        <v>-0.20502923272413492</v>
+      </c>
+      <c r="L137">
+        <f t="shared" si="5"/>
+        <v>-6.5854281120088787E-2</v>
+      </c>
+      <c r="M137">
+        <f t="shared" si="6"/>
+        <v>0.93626728617199417</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E138">
+        <v>130</v>
+      </c>
+      <c r="F138">
+        <v>132.5</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="1"/>
+        <v>0.87007579398600776</v>
+      </c>
+      <c r="H138">
+        <f t="shared" si="7"/>
+        <v>0.87007579398600776</v>
+      </c>
+      <c r="I138">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K138">
+        <f t="shared" si="4"/>
+        <v>-0.13917495160404614</v>
+      </c>
+      <c r="L138">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M138">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>51.822366199999998</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>36.259990414500002</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>0.99999997709400001</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>85</v>
       </c>
@@ -2225,8 +3209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2472,6 +3456,18 @@
       <c r="F8" t="s">
         <v>144</v>
       </c>
+      <c r="H8" t="s">
+        <v>155</v>
+      </c>
+      <c r="J8" t="s">
+        <v>156</v>
+      </c>
+      <c r="K8" t="s">
+        <v>157</v>
+      </c>
+      <c r="L8" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B9">
@@ -2486,6 +3482,9 @@
       <c r="F9">
         <v>9.6541376560700005</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B10">
@@ -2500,6 +3499,9 @@
       <c r="F10">
         <v>9.7910719438299996</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B11">
@@ -2514,6 +3516,9 @@
       <c r="F11">
         <v>10.219282849800001</v>
       </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B12">
@@ -2528,6 +3533,9 @@
       <c r="F12">
         <v>11.270183551000001</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B13">
@@ -2542,6 +3550,9 @@
       <c r="F13">
         <v>13.065030694300001</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B14">
@@ -2556,6 +3567,9 @@
       <c r="F14">
         <v>13.897168668100001</v>
       </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B15">
@@ -2570,6 +3584,9 @@
       <c r="F15">
         <v>13.344126789800001</v>
       </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B16">
@@ -2584,8 +3601,11 @@
       <c r="F16">
         <v>12.423934918900001</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>11.7433927738</v>
       </c>
@@ -2598,8 +3618,11 @@
       <c r="F17">
         <v>11.488009053600001</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>11.6203128987</v>
       </c>
@@ -2612,8 +3635,11 @@
       <c r="F18">
         <v>10.0512170664</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>11.2405482325</v>
       </c>
@@ -2626,8 +3652,11 @@
       <c r="F19">
         <v>9.0790765120200003</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>10.946996670900001</v>
       </c>
@@ -2640,8 +3669,11 @@
       <c r="F20">
         <v>8.6585545634500001</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>11.0616797118</v>
       </c>
@@ -2654,8 +3686,11 @@
       <c r="F21">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>10.852059370699999</v>
       </c>
@@ -2668,8 +3703,11 @@
       <c r="F22">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>9.5515696719799994</v>
       </c>
@@ -2682,8 +3720,11 @@
       <c r="F23">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>8.2545820193800008</v>
       </c>
@@ -2696,8 +3737,11 @@
       <c r="F24">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>7.2342957640699996</v>
       </c>
@@ -2710,8 +3754,11 @@
       <c r="F25">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>6.5247002737299997</v>
       </c>
@@ -2724,8 +3771,11 @@
       <c r="F26">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>6.0272153204499999</v>
       </c>
@@ -2738,8 +3788,11 @@
       <c r="F27">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>5.6665487986500001</v>
       </c>
@@ -2752,8 +3805,11 @@
       <c r="F28">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>5.4168816243000002</v>
       </c>
@@ -2766,8 +3822,11 @@
       <c r="F29">
         <v>-9.8999579077799993</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>5.2877781700600002</v>
       </c>
@@ -2779,6 +3838,9 @@
       </c>
       <c r="F30">
         <v>-9.8999579077799993</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3497,7 +4559,7 @@
         <v>7.5</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F14" si="1">(E3^($J$4-1))*EXP(-E3/$J$2)</f>
+        <f t="shared" ref="F3:F7" si="1">(E3^($J$4-1))*EXP(-E3/$J$2)</f>
         <v>6.705601108624041</v>
       </c>
       <c r="G3">
@@ -3815,15 +4877,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -3837,7 +4902,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>0.32241500000000001</v>
       </c>
@@ -3845,7 +4910,7 @@
         <v>0.32241500000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -3865,7 +4930,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0.36144700000000002</v>
       </c>
@@ -3873,7 +4938,7 @@
         <v>0.31065399999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -3893,12 +4958,61 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0.36144700000000002</v>
       </c>
       <c r="C6">
         <v>0.31065399999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9">
+        <v>0.31065399999999999</v>
+      </c>
+      <c r="D9">
+        <v>3.7159442120766349E-2</v>
+      </c>
+      <c r="E9">
+        <f>B9*EXP(D9)</f>
+        <v>0.32241489011133884</v>
+      </c>
+      <c r="G9">
+        <v>3.7159442120766349E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10">
+        <v>0.36144700000000002</v>
+      </c>
+      <c r="D10">
+        <v>-0.11427634866538093</v>
+      </c>
+      <c r="E10">
+        <f>B10*EXP(D10)</f>
+        <v>0.32241485015397275</v>
+      </c>
+      <c r="G10">
+        <v>-0.11427634866538093</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11">
+        <v>0.32241500000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3910,7 +5024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>

</xml_diff>